<commit_message>
fix fastq filedate in jp 092120
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_09.21.20.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_09.21.20.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Brent_Exp25_23_GTAC_35_SIC_Index2_08_CGCTACAATC_AAGCACGT_S18_R1_001.fastq.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">08.30.20</t>
+    <t xml:space="preserve">08.27.20</t>
   </si>
   <si>
     <t xml:space="preserve">H.BROWN</t>
@@ -320,8 +320,8 @@
   </sheetPr>
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -999,7 +999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>34</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>34</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>34</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>34</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>34</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>34</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
manual review of 4588
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_09.21.20.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_09.21.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="70">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">fastqFileName</t>
   </si>
   <si>
+    <t xml:space="preserve">MANUAL_REVIEW_101220</t>
+  </si>
+  <si>
     <t xml:space="preserve">09.02.20</t>
   </si>
   <si>
@@ -85,6 +88,9 @@
     <t xml:space="preserve">Brent_Exp25_4_GTAC_7_SIC_Index2_08_AGACTGAATC_AAGCACGT_S5_R1_001.fastq.gz</t>
   </si>
   <si>
+    <t xml:space="preserve">MANUAL_PASS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brent_Exp25_5_GTAC_8_SIC_Index2_08_CTTGGAAATC_AAGCACGT_S6_R1_001.fastq.gz</t>
   </si>
   <si>
@@ -182,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">Brent_Exp27_9_GTAC_51_SIC_Index2_06_CTCCCGAATC_GACCTTGT_S35_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL_FAIL</t>
   </si>
   <si>
     <t xml:space="preserve">Brent_Exp27_10_GTAC_52_SIC_Index2_06_GCCGTTTATC_GACCTTGT_S36_R1_001.fastq.gz</t>
@@ -318,17 +327,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="82.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -368,13 +379,16 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -383,13 +397,13 @@
         <v>4588</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>21.2</v>
@@ -401,15 +415,15 @@
         <v>8797182</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2</v>
@@ -418,13 +432,13 @@
         <v>4588</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>2.35</v>
@@ -436,15 +450,15 @@
         <v>3413224</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
@@ -453,13 +467,13 @@
         <v>4588</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>10.8</v>
@@ -471,15 +485,15 @@
         <v>8716271</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>4</v>
@@ -488,13 +502,13 @@
         <v>4588</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>6.87</v>
@@ -506,15 +520,18 @@
         <v>7416823</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>5</v>
@@ -523,13 +540,13 @@
         <v>4588</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>3.76</v>
@@ -541,15 +558,18 @@
         <v>7645462</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>6</v>
@@ -558,13 +578,13 @@
         <v>4588</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>5.3</v>
@@ -576,15 +596,15 @@
         <v>7553216</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>7</v>
@@ -593,13 +613,13 @@
         <v>4588</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>1.57</v>
@@ -611,15 +631,15 @@
         <v>10872849</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>8</v>
@@ -628,13 +648,13 @@
         <v>4588</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>22.4</v>
@@ -646,15 +666,15 @@
         <v>7068833</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>12</v>
@@ -663,13 +683,13 @@
         <v>4588</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>17.1</v>
@@ -681,15 +701,15 @@
         <v>7275284</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>13</v>
@@ -698,13 +718,13 @@
         <v>4588</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>2.57</v>
@@ -716,15 +736,15 @@
         <v>10479552</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>16</v>
@@ -733,13 +753,13 @@
         <v>4588</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>3.37</v>
@@ -751,15 +771,15 @@
         <v>7422146</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>17</v>
@@ -768,13 +788,13 @@
         <v>4588</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>6.56</v>
@@ -786,15 +806,15 @@
         <v>8540709</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>18</v>
@@ -803,13 +823,13 @@
         <v>4588</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>8.38</v>
@@ -821,15 +841,15 @@
         <v>8042588</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>19</v>
@@ -838,13 +858,13 @@
         <v>4588</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>1.49</v>
@@ -856,15 +876,15 @@
         <v>5506110</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>21</v>
@@ -873,13 +893,13 @@
         <v>4588</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>43.6</v>
@@ -891,15 +911,15 @@
         <v>8430712</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>22</v>
@@ -908,13 +928,13 @@
         <v>4588</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>62.9</v>
@@ -926,15 +946,15 @@
         <v>8572772</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>23</v>
@@ -943,13 +963,13 @@
         <v>4588</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>27.5</v>
@@ -961,15 +981,15 @@
         <v>7837403</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
@@ -978,13 +998,13 @@
         <v>4588</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>94.2</v>
@@ -996,15 +1016,15 @@
         <v>7432288</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>2</v>
@@ -1013,13 +1033,13 @@
         <v>4588</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>119</v>
@@ -1031,15 +1051,15 @@
         <v>7004200</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>3</v>
@@ -1048,13 +1068,13 @@
         <v>4588</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>24</v>
@@ -1066,15 +1086,15 @@
         <v>13956454</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>4</v>
@@ -1083,13 +1103,13 @@
         <v>4588</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>35.2</v>
@@ -1101,15 +1121,15 @@
         <v>7357291</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>5</v>
@@ -1118,13 +1138,13 @@
         <v>4588</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>21</v>
@@ -1136,15 +1156,15 @@
         <v>8315277</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>6</v>
@@ -1153,13 +1173,13 @@
         <v>4588</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>143</v>
@@ -1171,15 +1191,15 @@
         <v>7600411</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>7</v>
@@ -1188,13 +1208,13 @@
         <v>4588</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>81.5</v>
@@ -1206,15 +1226,15 @@
         <v>9388582</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>8</v>
@@ -1223,13 +1243,13 @@
         <v>4588</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>50.7</v>
@@ -1241,15 +1261,15 @@
         <v>8225970</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1</v>
@@ -1258,13 +1278,13 @@
         <v>4588</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>16.7</v>
@@ -1276,15 +1296,15 @@
         <v>9532904</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>2</v>
@@ -1293,13 +1313,13 @@
         <v>4588</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>8.67</v>
@@ -1311,15 +1331,15 @@
         <v>9489424</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>3</v>
@@ -1328,13 +1348,13 @@
         <v>4588</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>11</v>
@@ -1346,15 +1366,15 @@
         <v>11199294</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>4</v>
@@ -1363,13 +1383,13 @@
         <v>4588</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>20.4</v>
@@ -1381,15 +1401,15 @@
         <v>8732031</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>5</v>
@@ -1398,13 +1418,13 @@
         <v>4588</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>46.9</v>
@@ -1416,15 +1436,15 @@
         <v>7804640</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>6</v>
@@ -1433,13 +1453,13 @@
         <v>4588</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>16.8</v>
@@ -1451,15 +1471,15 @@
         <v>11042637</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>7</v>
@@ -1468,13 +1488,13 @@
         <v>4588</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>16.2</v>
@@ -1486,15 +1506,15 @@
         <v>8955279</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>8</v>
@@ -1503,13 +1523,13 @@
         <v>4588</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>15.5</v>
@@ -1521,15 +1541,15 @@
         <v>9652956</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>9</v>
@@ -1538,13 +1558,13 @@
         <v>4588</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>1.18</v>
@@ -1556,15 +1576,18 @@
         <v>1778922</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>10</v>
@@ -1573,13 +1596,13 @@
         <v>4588</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>8.66</v>
@@ -1591,15 +1614,15 @@
         <v>8707856</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>11</v>
@@ -1608,13 +1631,13 @@
         <v>4588</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>37.3</v>
@@ -1626,15 +1649,15 @@
         <v>8771886</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>12</v>
@@ -1643,13 +1666,13 @@
         <v>4588</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>45.3</v>
@@ -1661,15 +1684,15 @@
         <v>8670204</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>14</v>
@@ -1678,13 +1701,13 @@
         <v>4588</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>3.88</v>
@@ -1696,15 +1719,15 @@
         <v>8901341</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>15</v>
@@ -1713,13 +1736,13 @@
         <v>4588</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>19</v>
@@ -1731,15 +1754,15 @@
         <v>7649468</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>17</v>
@@ -1748,13 +1771,13 @@
         <v>4588</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>15.5</v>
@@ -1766,15 +1789,15 @@
         <v>8486185</v>
       </c>
       <c r="L41" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>18</v>
@@ -1783,13 +1806,13 @@
         <v>4588</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>22.9</v>
@@ -1801,15 +1824,15 @@
         <v>8254384</v>
       </c>
       <c r="L42" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>19</v>
@@ -1818,13 +1841,13 @@
         <v>4588</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>25.3</v>
@@ -1836,15 +1859,15 @@
         <v>9455887</v>
       </c>
       <c r="L43" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>20</v>
@@ -1853,13 +1876,13 @@
         <v>4588</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>47.1</v>
@@ -1871,15 +1894,15 @@
         <v>9712269</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>21</v>
@@ -1888,13 +1911,13 @@
         <v>4588</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>32.6</v>
@@ -1906,15 +1929,15 @@
         <v>7648415</v>
       </c>
       <c r="L45" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>22</v>
@@ -1923,13 +1946,13 @@
         <v>4588</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>21.1</v>
@@ -1941,15 +1964,15 @@
         <v>9480975</v>
       </c>
       <c r="L46" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>23</v>
@@ -1958,13 +1981,13 @@
         <v>4588</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>88.5</v>
@@ -1976,15 +1999,15 @@
         <v>7974154</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>24</v>
@@ -1993,13 +2016,13 @@
         <v>4588</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>6.65</v>
@@ -2011,7 +2034,7 @@
         <v>9507221</v>
       </c>
       <c r="L48" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding manual review notes to 4588 fastq 092120
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_09.21.20.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_09.21.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="70">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -329,8 +329,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,7 +338,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="82.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.83"/>
   </cols>
   <sheetData>
@@ -773,6 +773,9 @@
       <c r="L12" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="M12" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -1616,6 +1619,9 @@
       <c r="L36" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="M36" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -1791,6 +1797,9 @@
       <c r="L41" s="0" t="s">
         <v>62</v>
       </c>
+      <c r="M41" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -1965,6 +1974,9 @@
       </c>
       <c r="L46" s="0" t="s">
         <v>67</v>
+      </c>
+      <c r="M46" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
finishing manual review of 4588
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_09.21.20.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_09.21.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="70">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -329,8 +329,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M45" activeCellId="0" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1940,6 +1940,9 @@
       <c r="L45" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="M45" s="0" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">

</xml_diff>